<commit_message>
Ready for EDM meeting 2nd Feb 2021
</commit_message>
<xml_diff>
--- a/n_splitting.xlsx
+++ b/n_splitting.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samuelgrant/Documents/gm2/EDM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{910C98C1-3389-A44D-B29A-6C1EAAA4C239}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B65CF1B0-4DB2-0142-B50B-4DFF0D6CF9DF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{F508F9FE-51F7-4B41-95B3-0CA03A1D87EF}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
   <si>
     <t xml:space="preserve">n </t>
   </si>
@@ -67,6 +67,12 @@
   </si>
   <si>
     <t>n20-n10</t>
+  </si>
+  <si>
+    <t>B field</t>
+  </si>
+  <si>
+    <t>E field</t>
   </si>
 </sst>
 </file>
@@ -105,9 +111,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -425,7 +432,7 @@
   <dimension ref="A1:R22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R20" sqref="R20"/>
+      <selection activeCell="J13" sqref="H1:J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -436,7 +443,7 @@
     <col min="5" max="5" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
@@ -490,7 +497,10 @@
         <v>6</v>
       </c>
       <c r="I2" t="s">
-        <v>8</v>
+        <v>11</v>
+      </c>
+      <c r="J2" t="s">
+        <v>12</v>
       </c>
       <c r="K2" t="s">
         <v>6</v>
@@ -536,6 +546,10 @@
         <f>(1/(H3^2-$F$20))-(1/(H3^2-$F$16))</f>
         <v>2.6903416733925205</v>
       </c>
+      <c r="J3">
+        <f>($F$20/(I3^2-$F$20))-($F$16/(I3^2-$F$16))</f>
+        <v>3.3473514153240218E-3</v>
+      </c>
       <c r="K3">
         <v>0</v>
       </c>
@@ -583,25 +597,29 @@
         <f t="shared" ref="I4:I13" si="2">(1/(H4^2-$F$20))-(1/(H4^2-$F$16))</f>
         <v>2.8781466374734777E-2</v>
       </c>
+      <c r="J4">
+        <f t="shared" ref="J4:J13" si="3">($F$20/(I4^2-$F$20))-($F$16/(I4^2-$F$16))</f>
+        <v>2.2688799121175496E-3</v>
+      </c>
       <c r="K4">
         <v>1</v>
       </c>
       <c r="L4">
-        <f t="shared" ref="L4:L13" si="3">(1/(K4^2-$F$22))-(1/(K4^2-$F$16))</f>
+        <f t="shared" ref="L4:L13" si="4">(1/(K4^2-$F$22))-(1/(K4^2-$F$16))</f>
         <v>4.374978681247943E-2</v>
       </c>
       <c r="N4">
         <v>1</v>
       </c>
       <c r="O4">
-        <f t="shared" ref="O4:O13" si="4">(1/(N4^2-$F$22))-(1/(N4^2-$F$12))</f>
+        <f t="shared" ref="O4:O13" si="5">(1/(N4^2-$F$22))-(1/(N4^2-$F$12))</f>
         <v>7.1087591962041508E-2</v>
       </c>
       <c r="Q4">
         <v>1</v>
       </c>
       <c r="R4">
-        <f t="shared" ref="R4:R13" si="5">(1/(Q4^2-$F$22))-(1/(Q4^2-$F$3))</f>
+        <f t="shared" ref="R4:R13" si="6">(1/(Q4^2-$F$22))-(1/(Q4^2-$F$3))</f>
         <v>0.12785183147463464</v>
       </c>
     </row>
@@ -630,25 +648,29 @@
         <f t="shared" si="2"/>
         <v>1.5471785765549528E-3</v>
       </c>
+      <c r="J5">
+        <f t="shared" si="3"/>
+        <v>6.440368253368689E-6</v>
+      </c>
       <c r="K5">
         <v>2</v>
       </c>
       <c r="L5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.3278222339218058E-3</v>
       </c>
       <c r="N5">
         <v>2</v>
       </c>
       <c r="O5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.8564707854035762E-3</v>
       </c>
       <c r="Q5">
         <v>2</v>
       </c>
       <c r="R5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>7.2298809729409719E-3</v>
       </c>
     </row>
@@ -667,25 +689,29 @@
         <f t="shared" si="2"/>
         <v>2.9756811654829685E-4</v>
       </c>
+      <c r="J6">
+        <f t="shared" si="3"/>
+        <v>2.3822155714725568E-7</v>
+      </c>
       <c r="K6">
         <v>3</v>
       </c>
       <c r="L6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4.4694516690339803E-4</v>
       </c>
       <c r="N6">
         <v>3</v>
       </c>
       <c r="O6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>7.429424060217682E-4</v>
       </c>
       <c r="Q6">
         <v>3</v>
       </c>
       <c r="R6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.4032567237696747E-3</v>
       </c>
     </row>
@@ -710,25 +736,29 @@
         <f t="shared" si="2"/>
         <v>9.3285067279041956E-5</v>
       </c>
+      <c r="J7">
+        <f t="shared" si="3"/>
+        <v>2.3411636851378148E-8</v>
+      </c>
       <c r="K7">
         <v>4</v>
       </c>
       <c r="L7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.4003156425383689E-4</v>
       </c>
       <c r="N7">
         <v>4</v>
       </c>
-      <c r="O7">
-        <f t="shared" si="4"/>
+      <c r="O7" s="2">
+        <f t="shared" si="5"/>
         <v>2.3304042206197251E-4</v>
       </c>
       <c r="Q7">
         <v>4</v>
       </c>
       <c r="R7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4.4130679434106757E-4</v>
       </c>
     </row>
@@ -747,25 +777,29 @@
         <f t="shared" si="2"/>
         <v>3.8046795397150834E-5</v>
       </c>
+      <c r="J8">
+        <f t="shared" si="3"/>
+        <v>3.8944274471930385E-9</v>
+      </c>
       <c r="K8">
         <v>5</v>
       </c>
       <c r="L8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5.7097257973086346E-5</v>
       </c>
       <c r="N8">
         <v>5</v>
       </c>
       <c r="O8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>9.5072051095157484E-5</v>
       </c>
       <c r="Q8">
         <v>5</v>
       </c>
       <c r="R8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.802531337432578E-4</v>
       </c>
     </row>
@@ -784,25 +818,29 @@
         <f t="shared" si="2"/>
         <v>1.8305756159860131E-5</v>
       </c>
+      <c r="J9">
+        <f t="shared" si="3"/>
+        <v>9.0153529086478557E-10</v>
+      </c>
       <c r="K9">
         <v>6</v>
       </c>
       <c r="L9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.7467664168001615E-5</v>
       </c>
       <c r="N9">
         <v>6</v>
       </c>
       <c r="O9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4.5749380048216298E-5</v>
       </c>
       <c r="Q9">
         <v>6</v>
       </c>
       <c r="R9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>8.6795588437951765E-5</v>
       </c>
     </row>
@@ -821,25 +859,29 @@
         <f t="shared" si="2"/>
         <v>9.8672207731673178E-6</v>
       </c>
+      <c r="J10">
+        <f t="shared" si="3"/>
+        <v>2.6193713864586243E-10</v>
+      </c>
       <c r="K10">
         <v>7</v>
       </c>
       <c r="L10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.4804404045633962E-5</v>
       </c>
       <c r="N10">
         <v>7</v>
       </c>
       <c r="O10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.4662108609067868E-5</v>
       </c>
       <c r="Q10">
         <v>7</v>
       </c>
       <c r="R10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4.6807221463992382E-5</v>
       </c>
     </row>
@@ -858,25 +900,29 @@
         <f t="shared" si="2"/>
         <v>5.7787536974496234E-6</v>
       </c>
+      <c r="J11">
+        <f t="shared" si="3"/>
+        <v>8.9841245554111993E-11</v>
+      </c>
       <c r="K11">
         <v>8</v>
       </c>
       <c r="L11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8.6697316848440009E-6</v>
       </c>
       <c r="N11">
         <v>8</v>
       </c>
       <c r="O11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.4444219618943432E-5</v>
       </c>
       <c r="Q11">
         <v>8</v>
       </c>
       <c r="R11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2.7421245218609003E-5</v>
       </c>
     </row>
@@ -895,25 +941,29 @@
         <f t="shared" si="2"/>
         <v>3.605411554752358E-6</v>
       </c>
+      <c r="J12">
+        <f t="shared" si="3"/>
+        <v>3.4971803231087506E-11</v>
+      </c>
       <c r="K12">
         <v>9</v>
       </c>
       <c r="L12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5.4089063307241614E-6</v>
       </c>
       <c r="N12">
         <v>9</v>
       </c>
       <c r="O12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>9.0122154228749335E-6</v>
       </c>
       <c r="Q12">
         <v>9</v>
       </c>
       <c r="R12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.7111983270774039E-5</v>
       </c>
     </row>
@@ -932,25 +982,29 @@
         <f t="shared" si="2"/>
         <v>2.3644620301792318E-6</v>
       </c>
+      <c r="J13">
+        <f t="shared" si="3"/>
+        <v>1.5040857448411771E-11</v>
+      </c>
       <c r="K13">
         <v>10</v>
       </c>
       <c r="L13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3.5471120494717095E-6</v>
       </c>
       <c r="N13">
         <v>10</v>
       </c>
       <c r="O13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5.9104573947275918E-6</v>
       </c>
       <c r="Q13">
         <v>10</v>
       </c>
       <c r="R13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.1223905637675405E-5</v>
       </c>
     </row>

</xml_diff>